<commit_message>
Aggiornamento README e altri file
</commit_message>
<xml_diff>
--- a/tasks_tesi.xlsx
+++ b/tasks_tesi.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinarusso/tesi_russo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E02D2D8-71E7-204B-B7BB-C194E016766E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB60065A-E588-D74E-986F-7A4A22192F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12320" yWindow="820" windowWidth="17060" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17480" yWindow="760" windowWidth="11860" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$181</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$189</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="216">
   <si>
     <t>Context</t>
   </si>
@@ -109,9 +109,6 @@
     <t>This sheet presents data related to Pump, Valve and Generator.</t>
   </si>
   <si>
-    <t>Add a "Sum" column to the right of each table and fill it with the sum of each row's values.</t>
-  </si>
-  <si>
     <t>This sheet presents  two tables and an image.</t>
   </si>
   <si>
@@ -227,12 +224,6 @@
     <t>1_58032_answer.xlsx</t>
   </si>
   <si>
-    <t>Replace all empty cells in all tables with the string 'MISSING'.</t>
-  </si>
-  <si>
-    <t>Replace all empty cells in all tables with the string 'MISSING'. Delete the "In role in 6 Months?" column.</t>
-  </si>
-  <si>
     <t>1_59129_input.xlsx</t>
   </si>
   <si>
@@ -246,6 +237,457 @@
   </si>
   <si>
     <t>1_CF_12429_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_312-46_answer.xlsx</t>
+  </si>
+  <si>
+    <t>In all the tables, delete all the rows where you find a "blank" cell.</t>
+  </si>
+  <si>
+    <t>1_49939_answer.xlsx</t>
+  </si>
+  <si>
+    <t>In the first table "DATA Table" add a new column "TOTAL" and compute the sum of the last seven columns. In the second table, find the "Emp code" with the highest "Total" value and highlight it in green.</t>
+  </si>
+  <si>
+    <t>1_45944_answer.xlsx</t>
+  </si>
+  <si>
+    <t>InsuranceCompanyFinancialExpenseDynamicAnalysisTable1(1).xlsx</t>
+  </si>
+  <si>
+    <t>1_CF_4909_answer.xlsx</t>
+  </si>
+  <si>
+    <t>BankDepositInterestRates.xlsx</t>
+  </si>
+  <si>
+    <t>1_50811_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_46646_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_575-16_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_409-45_input.xlsx</t>
+  </si>
+  <si>
+    <t>InventoryManagementSheetforInboundandOutbound.xlsx</t>
+  </si>
+  <si>
+    <t>ProjectStatisticsTable1.xlsx</t>
+  </si>
+  <si>
+    <t>83.xlsx</t>
+  </si>
+  <si>
+    <t>1_45937_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_37456_answer.xlsx</t>
+  </si>
+  <si>
+    <t>FinancialAccountingSheet(AutoSummaryandQueryable)1.xlsx</t>
+  </si>
+  <si>
+    <t>1_50816_answer.xlsx</t>
+  </si>
+  <si>
+    <t>Long-termLoanRepaymentPlan.xlsx</t>
+  </si>
+  <si>
+    <t>1_49196_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_208-20_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_404-14_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_58296_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_183-8_answer.xlsx</t>
+  </si>
+  <si>
+    <t>AthleticsCompetitionScoreboard1.xlsx</t>
+  </si>
+  <si>
+    <t>1_59055_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_444-14_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_55860_answer.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort all the tables in a descending order for the "START DATE" column. </t>
+  </si>
+  <si>
+    <t>For all pathways marked as “YES” under “APPLICABLE”, calculate the average value for each contaminant (Benzene, Toluene, etc.) among valid numeric entries, and compare these averages to the corresponding “CRITERIA” values below. Highlight any average that exceeds its criterion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the highest "result in %" that the "Employee Name" "Jhon Smith" reached in the "Year" "2016"? Highlight the "result in %" cell and the corresponding month in yellow. </t>
+  </si>
+  <si>
+    <t>Summarize by "Workstation" and "Product Part Number":in a new sheet, create a summary table listing, for each "Workstation" × "Product Part Number", the total "Production Quantity", total "Defective Quantity", weighted "Defect Rate", and weighted "Yield Rate". Sort by weighted "Defect Rate" descending.</t>
+  </si>
+  <si>
+    <t>Consistency audit: Find any inconsistencies where the same term’s adjusted/execution rate differs between sheets; list conflicts in a “Conflicts” table with Sheet, Item, Term, Rate1, Rate2. Write the conflicts into a new “Conflicts” sheet.</t>
+  </si>
+  <si>
+    <t>Multi-criteria retrieval: Given a Rep and Client in the lower table, return the corresponding commission % from the upper table by matching on the Rep name across Rep 1–Rep 5 and the Client in the “Casino Client” column; populate the % column for all lower rows.</t>
+  </si>
+  <si>
+    <t>Allocation sum validation: For each row, sum all "%" fields across "Rep 1".."Rep 5" and flag rows where the total is not within [0.99, 1.01] as “Allocation Error” in red</t>
+  </si>
+  <si>
+    <t>Add a "Sum" column to the right of each table and fill it with the sum of each rows values.</t>
+  </si>
+  <si>
+    <t>Replace all empty cells in all tables with the string "MISSING". Delete the "In role in 6 Months?" column.</t>
+  </si>
+  <si>
+    <t>Replace all empty cells in all tables with the string "MISSING".</t>
+  </si>
+  <si>
+    <t>Best/Worst months: Identify the month with the maximum and minimum “result in %”; color the maximum in green and the minimum in orange in the result row.</t>
+  </si>
+  <si>
+    <t>1_46646_answer copy.xlsx</t>
+  </si>
+  <si>
+    <t>Consolidate segmented tables: In the “DATA” sheet, detect each repeated header block (date, id, batch, q1, q2), extract their data rows, and vertically stack them into a single normalized table with the same five columns. Preserve dates and values as-is. Write the result into the “desired result” sheet, keeping blank separator rows exactly as shown.</t>
+  </si>
+  <si>
+    <t>In the “Inventory Statistics Information” section, for each Product Name present in the main table, fill “Inbound Quantity”, “Outbound Quantity”, and “Inventory Quantity”. Apply red background fill to any “Inventory Quantity” cell where the value is negative.</t>
+  </si>
+  <si>
+    <t>Compute for each project whether Actual ("Estimated End Date" − "Project Start Date") equals "Proposed Duration"; if the absolute difference &gt; 1 day, mark the row in orange.</t>
+  </si>
+  <si>
+    <t>Compute the difference between "Total Amount Due" and "Actual Total Amount Received" and write it in red under the "Actual Total Amount Received" cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For each non complete row in the top table, compute the correct percentage in the “%” column by looking up the "kms" band and "Category" in the rate grid.
+</t>
+  </si>
+  <si>
+    <t>From the left event log ("Date", "Time", "Product", "Sales"), aggregate to daily totals per Product and populate the “Optimal Table” ("Date" × Products A–D). If a product has no sales on a date, fill 0.</t>
+  </si>
+  <si>
+    <t>In a new sheet named "summary", Create a two-column summary table listing top 5 income "Category" and top 5 expenditure "Category" by amount for the selected month.</t>
+  </si>
+  <si>
+    <t>Extract the reward name from “Items” (strip stub counts in parentheses) into a helper column, and produce a compact list of all unique reward types with first-unlock point threshold.</t>
+  </si>
+  <si>
+    <t>Compare each period’s computed monthly payments against “Monthly Salary Repayment Limit” and “Each Extra Salary Income Repayment Limit”; mark “Repayment OK/NOT OK” accordingly in “Repayment Judgment.”</t>
+  </si>
+  <si>
+    <t>For each row, compute “Start finishing” to “End finishing” duration in hours and in days (two new columns). Highlight negative or zero durations in red background.</t>
+  </si>
+  <si>
+    <t>For each symbol/date row in “Actual Result,” find the matching row in “Expected Result” (same symbol and "DATE") and compare "OPEN", "SIGNAL", and "R DAYS"; highlight mismatches in yellow and write a new “Match” column with “OK/DIFF.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only keep the most recent “NO PAID” invoice row if any exists for the NAME; otherwise keep the last “PAID” row. Ensure one output row per NAME in the new sheet“result2”.
+</t>
+  </si>
+  <si>
+    <t>Recalculate the Sum for each (Month Start, Month End) window from the Date/Amount list using inclusive date range and write the rounded result to two decimals. Highlight discrepancies &gt; 0.01 with yellow fill.</t>
+  </si>
+  <si>
+    <t>Build a compact summary at the bottom listing, per "OEM", the max yearly generation and its "FY", and rank "OEM"s by total generation descending.</t>
+  </si>
+  <si>
+    <t>If multiple classes share the same "Total Points", assign them the same rank (dense ranking), and skip subsequent numbers accordingly. Highlight tied rows in light yellow.</t>
+  </si>
+  <si>
+    <t>For each code block (KT1, KR4, JLP2, BR1), verify that the two “Sales Allocation” rows and the single “Check” row match numerically (left and right amounts equal). Highlight the “Check” amount in green if both sides match; in red if they differ.</t>
+  </si>
+  <si>
+    <t>In “Print File” sheet,  for each “Record no” listed in the right-hand columns, look it up in either “Basic Master” or “Data” (Tab Name indicated in the middle column). Populate the far-right column with the same "Record no" if found; otherwise write “Not Found” and highlight in red.</t>
+  </si>
+  <si>
+    <t>Using the top matrix ("Code", "Name", "Detail", "Period" 1–12), fill the bottom transactional table so that for each Date/Period/Code row the columns “Funeral,” “Medical AID,” “Trade Union,” and “Others” are populated from the corresponding period values; leave blanks where details are missing.</t>
+  </si>
+  <si>
+    <t>1_82-38_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_32612_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_13-1_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_41937_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_402-43_input.xlsx</t>
+  </si>
+  <si>
+    <t>ElectronicInvoiceRegistrationDetailStatisticsTable.xlsx</t>
+  </si>
+  <si>
+    <t>InboundandOutboundInventory(4).xlsx</t>
+  </si>
+  <si>
+    <t>1237(2).xlsx</t>
+  </si>
+  <si>
+    <t>1_54513_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_43657_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_52292_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_3911_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_42798_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_41297_answer.xlsx</t>
+  </si>
+  <si>
+    <t>OrderCostCalculationTable1.xlsx</t>
+  </si>
+  <si>
+    <t>1_50452_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_2212_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_58829_answer.xlsx</t>
+  </si>
+  <si>
+    <t>FinancialProfitAnalysisTable.xlsx</t>
+  </si>
+  <si>
+    <t>1_71-30_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_530-28_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_53994_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_53161_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_57989_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_118-10_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_51030_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_42217_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_15825_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_22-47_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_32468_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_CF_11177_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_42216_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_17049_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_50442_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_57090_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_62-3_input.xlsx</t>
+  </si>
+  <si>
+    <t>1_55883_answer.xlsx</t>
+  </si>
+  <si>
+    <t>1_41-47_input.xlsx</t>
+  </si>
+  <si>
+    <t>Ensure each invoice/line in the sheet “SH1” exists in yhe sheet “DATA” (match by "INVOICE NO" and "CODE"); highlight missing matches in red in SH1. Conversely, flag in the sheet “DATA” any invoice not present in the sheet “SH1” in a small new “Unmatched in SH1” list.</t>
+  </si>
+  <si>
+    <t>Flag rows where "TOTAL HOURS" &lt; 04:00:00 in orange as “Under 4h” and rows &gt; 04:30:00 in purple as “Over 4.5h”. Provide a summary of counts by category at the bottom.</t>
+  </si>
+  <si>
+    <t>For each section in the sheet “RANGES” ("STAGE", "DATA", "OPERATION"), group by "DATE" and "REF" and compute "AMOUNTS" = sum of AMOUNTS. Populate the corresponding section in  the sheet “LISTS” (STAGE/DATA/OPERATION tables) with one row per (DATE, REF) and a "TOTAL" line = sum of "AMOUNTS" per section.</t>
+  </si>
+  <si>
+    <t>Using the list of records above the “Goal” area, mark an “x” in the goal matrix for each combination where a row exists with given "Atype" (T20), "Ccode", "Texture" (BLANK/MATT), and "Quality" (P/C/Y). Preserve existing x marks and fill any missing ones.</t>
+  </si>
+  <si>
+    <t>Provide a small summary table listing counts of backed, added, and unbacked combinations.</t>
+  </si>
+  <si>
+    <t>1_41937_input copy.xlsx</t>
+  </si>
+  <si>
+    <t>Verify the total number of output rows of the below table equals the sum of "COUNT" of the above table; if not, output a warning “Row count mismatch” beneath the expanded table.</t>
+  </si>
+  <si>
+    <t>For each detailed row, ensure “Electronic Invoice Type” is one of the declared types and “Whether Sent to Customer” is 0/1; highlight invalid or blank entries in yellow.</t>
+  </si>
+  <si>
+    <t>Highlight in green the cells with the highest "Inbound" and "Outbound" Monthly Totals.</t>
+  </si>
+  <si>
+    <t>In the " Team Building Cost Budget Summary (Two Times) " table, highlight in pink the highest value in row "Budget Summary":</t>
+  </si>
+  <si>
+    <t>For each date, verify at least one assignment exists. Fill in red the ucovered dates.</t>
+  </si>
+  <si>
+    <t>Create a compact table listing, for each quantity in {12, 24, 36, 48, 60, 72, 84, 96}, the option that yields the lowest Final Unit Cost and the corresponding cost; highlight the best option cell in green.</t>
+  </si>
+  <si>
+    <t>Add a summary table below with "total cost per region" (sum across roles) and" total cost per role" (min across regions × hours). Bold the cheapest region per role.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oreder the above table for descendind "NetSalary".
+</t>
+  </si>
+  <si>
+    <t>For each assignment (date) per "Item No.", ensure the date lies within ["Start Date", "End Date"]; highlight violations in red and list them in a “Window Violations” section.</t>
+  </si>
+  <si>
+    <t>Merge and align series: Combine “Column A” and “Column B” into a single chronological series with columns ("Date", "Value_A", "Value_B"). Where a Date exists in one series but not the other, leave the missing side blank.</t>
+  </si>
+  <si>
+    <t>Add columns “Unit Margin" = ("Order Amount" / "Order Quantity") − Unit Total Cost and “Margin %" = "Profit Amount" / "Order Amount".</t>
+  </si>
+  <si>
+    <t>Rank "Dir" by number of assignments; flag those below the 25th percentile as “Under-assigned” and above the 75th percentile as “Over-assigned.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a two-column mapping table that links each raw "DATE" to its corresponding "MONTHS" bucket, preserving original formats; flag "DATE" entries that don’t map to any MONTHS value.
+</t>
+  </si>
+  <si>
+    <t>Tag" MONTHS" rows with Nos. outside the interquartile range as “Outlier” in a new column; do not alter source values.</t>
+  </si>
+  <si>
+    <t>1_2212_answer copy.xlsx</t>
+  </si>
+  <si>
+    <t>For each category ("Main Income", "Main Cost", "Tax", "Period Expenses"), mark months where “This Year” exceeds the 75th percentile of its own yearly distribution as “Peak” and below 25th percentile as “Trough.”</t>
+  </si>
+  <si>
+    <t>Build a compact panel with “Best Month,” “Worst Month,” “Most volatile month” (highest absolute growth), and “Stable month” (lowest absolute growth), per metric.</t>
+  </si>
+  <si>
+    <t>FinancialProfitAnalysisTable copy.xlsx</t>
+  </si>
+  <si>
+    <t>For each "PRODUCT NO", populate the right-hand ladder columns as alternating pairs of "PRICE 1" and "PRICE 2"</t>
+  </si>
+  <si>
+    <t>Using the selected year’s band table, record the “MORE THAN–BUT NOT MORE THAN” interval that contains the car’s “co2 g” value in a new “CO2 Band” column.</t>
+  </si>
+  <si>
+    <t>Using the header "Total Time(Mins)" (M1/M2/M3 SETUP/RUN), tag any batch where a machine’s allocated time exceeds 40% of its header total with red and highlight with yellow those machine entries.</t>
+  </si>
+  <si>
+    <t>For each "Agent", identify continuous gaps of at least 60 minutes with no assigned intervals; add a “Gaps (mins)” tally per agent.</t>
+  </si>
+  <si>
+    <t>In “Synthese,” add a column “Total Week Duties” = sum across weekday columns; sort drivers descending and bold the top 3.</t>
+  </si>
+  <si>
+    <t>1_57989_answer copy.xlsx</t>
+  </si>
+  <si>
+    <t>Highlight any day where a driver has “hk” on three consecutive days.</t>
+  </si>
+  <si>
+    <t>For each Ledger, identify exact duplicate rows and delete them.</t>
+  </si>
+  <si>
+    <t>Within each "Ledger" in the "Result" sheet, compute a non-editing helper list of cumulative totals over time; append a “Summary” line per Ledger with first date, last date, entries count, and final balance.</t>
+  </si>
+  <si>
+    <t>1_118-10_answer copy.xlsx</t>
+  </si>
+  <si>
+    <t>For each “Reason,” identify the top 3 weeks with the highest counts across the long weekly panel; mark those week columns with a light green background in both panels for that reason.</t>
+  </si>
+  <si>
+    <t>Identify the right-side table and Copy this entire table (including the header row) into a new worksheet named “Sheet2”, preserving column order and values. Leave the original sheet unchanged.</t>
+  </si>
+  <si>
+    <t>Create a unified table with columns ("Date", "A_observed", "A_modelled", "A_infilled"), matching by Date and leaving blanks where a group has no value.</t>
+  </si>
+  <si>
+    <t>Populate the single empty table with columns ("ITEM", "NAME", "REF") by stacking all blocks found in "sheet1".</t>
+  </si>
+  <si>
+    <t>Join "INCOME" “MONTH"/"Total” with "12 MONTH DISCOUNT FROM POINT OF SALE" “MONTH"/"Total” by month into a table ("Month", "Income_Total", "Discount_Total"); keep both signs as‑is.</t>
+  </si>
+  <si>
+    <t>List dates where any of the three windows changed compared to the previous day.</t>
+  </si>
+  <si>
+    <t>For each Year‑Month, compute count of valid days in Group A and in Group B; highlight cells months with coverage &lt; 80% in orange.</t>
+  </si>
+  <si>
+    <t>1_42216_answer copy.xlsx</t>
+  </si>
+  <si>
+    <t>From "Group B" table, delete the rows with sentinel values like "−99999" or “NA” or "0".</t>
+  </si>
+  <si>
+    <t>Duplicate the "Output (Filtered List)" table in a new sheet called "Output".</t>
+  </si>
+  <si>
+    <t>In both the tables, delete the rows that have the second column ("Recent Date" and "LSPM report shared date" respectively) empy.</t>
+  </si>
+  <si>
+    <t>In the second table, underline the year that has a higher count.</t>
+  </si>
+  <si>
+    <t>Within the "CALCS" sheet, use the "TIME CALCS" table to calculate the time slot with the highest number of ENTRIES and report its average trade time.</t>
+  </si>
+  <si>
+    <t>For each "BATCH", compute the net sum of "IMPORT" minus "EXPORT" for the year 2010. Return the top 5 batches with the highest net inflow.</t>
+  </si>
+  <si>
+    <t>Extract all rows from 2023 and calculate the monthly total of "IMPORT". Write a table with month and total import.</t>
+  </si>
+  <si>
+    <t>1_62-3_input copy.xlsx</t>
+  </si>
+  <si>
+    <t>In the "Holiday 01APR21 - 31MAR22" sheet, generate a summary for each "NAME": total "HOLIDAY (H)", "HALF DAY (HD)", and "SICK (S)" days, including percentage of each over all working days.</t>
+  </si>
+  <si>
+    <t>From the "OUT CAS" sheet, summarize per "ITEM" the total "PUR PURCHASE", total "PUR PAID" and compare them as a bar chart.</t>
   </si>
 </sst>
 </file>
@@ -641,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +1124,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -695,7 +1137,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -708,7 +1150,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -721,7 +1163,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -734,7 +1176,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -757,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>22</v>
@@ -773,7 +1215,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -783,10 +1225,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -796,711 +1238,1006 @@
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+    <row r="33" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
+    <row r="34" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+    <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
+      <c r="C35" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="C36" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
+      <c r="C37" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+    <row r="39" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
+    <row r="40" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
+    <row r="41" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
+    <row r="42" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
+    <row r="43" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
+    <row r="44" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
+    <row r="45" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
+    <row r="46" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="C49" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
+    </row>
+    <row r="50" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="7"/>
+    </row>
+    <row r="53" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
+    <row r="54" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="7"/>
+    <row r="55" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>94</v>
+      </c>
       <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
+    <row r="56" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+      <c r="C56" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="7"/>
+    <row r="57" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="7"/>
+    <row r="58" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="C58" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="7"/>
+    <row r="59" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>166</v>
+      </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="7"/>
+    <row r="60" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="7"/>
+    <row r="61" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="7"/>
+    <row r="62" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="7"/>
+    <row r="63" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="7"/>
+    <row r="64" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
+        <v>132</v>
+      </c>
       <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="7"/>
+    <row r="65" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
+        <v>133</v>
+      </c>
       <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="7"/>
+    <row r="66" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="7"/>
+    <row r="67" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
+        <v>135</v>
+      </c>
       <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="7"/>
+    <row r="68" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="7"/>
+    <row r="69" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="7"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
+      <c r="C70" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
+    <row r="71" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
+      <c r="C71" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="7"/>
+    </row>
+    <row r="72" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A72" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="7"/>
+    <row r="73" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="7"/>
+    <row r="74" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
+        <v>184</v>
+      </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="7"/>
+    <row r="75" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
+        <v>142</v>
+      </c>
       <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
+      <c r="C75" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="7"/>
+    <row r="76" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
+      <c r="C76" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="7"/>
+    <row r="77" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
+      <c r="C77" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="7"/>
+    <row r="78" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
+        <v>187</v>
+      </c>
       <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="7"/>
+    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
+        <v>145</v>
+      </c>
       <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="7"/>
+    <row r="80" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="7"/>
+    <row r="81" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
+        <v>147</v>
+      </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
+      <c r="C81" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="7"/>
+    <row r="82" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>148</v>
+      </c>
       <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
+      <c r="C82" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="7"/>
+    <row r="83" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A83" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
+      <c r="C83" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="7"/>
+    <row r="84" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
+      <c r="C84" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="7"/>
+    <row r="85" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
+      <c r="C85" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="7"/>
+    <row r="86" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
+      <c r="C86" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="7"/>
+    <row r="87" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
+        <v>151</v>
+      </c>
       <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+      <c r="C87" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="7"/>
+    <row r="88" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A88" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
+      <c r="C88" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="7"/>
+    <row r="89" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A89" s="7" t="s">
+        <v>153</v>
+      </c>
       <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
+      <c r="C89" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="7"/>
+    <row r="90" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="7" t="s">
+        <v>154</v>
+      </c>
       <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="7"/>
+    <row r="91" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A91" s="7" t="s">
+        <v>155</v>
+      </c>
       <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>202</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="7"/>
+    <row r="92" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="7" t="s">
+        <v>156</v>
+      </c>
       <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>203</v>
+      </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="7"/>
+    <row r="93" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
+        <v>157</v>
+      </c>
       <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
+      <c r="C93" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="7"/>
+    <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+      <c r="C94" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="7"/>
+    <row r="95" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
+      <c r="C95" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="7"/>
+    <row r="96" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
+      <c r="C96" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="D96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="7"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
+      <c r="C97" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="7"/>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A98" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
+      <c r="C98" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="7"/>
+    <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" s="7" t="s">
+        <v>213</v>
+      </c>
       <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
+      <c r="C99" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="7"/>
+    <row r="100" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A100" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>214</v>
+      </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="7"/>
+    <row r="101" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A101" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
+      <c r="C101" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
     </row>
@@ -1523,14 +2260,12 @@
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
@@ -1588,7 +2323,7 @@
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
     </row>
-    <row r="114" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -1644,7 +2379,7 @@
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -1686,7 +2421,7 @@
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
     </row>
-    <row r="128" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="7"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -1742,7 +2477,7 @@
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="7"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -2064,6 +2799,62 @@
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
     </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="7"/>
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="7"/>
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+      <c r="E183" s="3"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="7"/>
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="7"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="7"/>
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="7"/>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="7"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="7"/>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
+      <c r="E189" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>